<commit_message>
Fixed error in test cases
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbaird\Source\Repos\DipUnitTestEx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Magnus Servio/Users/tim/Repos/DipSWDTestExercises/DipSWDTestExercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1082CD-D472-D14A-8422-2A234D6BDFCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="645" windowWidth="26460" windowHeight="17880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +107,6 @@
     <t>getFuelRemaining() = 50</t>
   </si>
   <si>
-    <t>vBus.maxPassengers = 25</t>
-  </si>
-  <si>
     <t>You complete</t>
   </si>
   <si>
@@ -196,9 +194,6 @@
   <si>
     <t>Exception with message containing Out of Fuel
 0 litres of fuel remianing</t>
-  </si>
-  <si>
-    <t>check maxPassengers = 25</t>
   </si>
   <si>
     <t>After second call
@@ -248,12 +243,18 @@
   </si>
   <si>
     <t>NOTE:   Write One Empty Test Called  Test_To_Ignore , the test can be empty, but ensure you place an ignore flag before the test</t>
+  </si>
+  <si>
+    <t>check maxPassengers = 1</t>
+  </si>
+  <si>
+    <t>vBus.maxPassengers = 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,29 +623,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -664,27 +665,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -692,19 +693,19 @@
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -712,19 +713,19 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -732,19 +733,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -752,19 +753,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -772,19 +773,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -792,19 +793,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -812,39 +813,39 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -852,19 +853,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,19 +873,19 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -892,19 +893,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -912,19 +913,19 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -932,39 +933,39 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -972,19 +973,19 @@
         <v>12</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -992,19 +993,19 @@
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1012,39 +1013,39 @@
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1052,19 +1053,19 @@
         <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1072,39 +1073,39 @@
         <v>14</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1112,19 +1113,19 @@
         <v>12</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1132,19 +1133,19 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1152,7 +1153,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1160,9 +1161,9 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1170,7 +1171,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1178,7 +1179,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1186,7 +1187,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1194,7 +1195,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1202,7 +1203,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1210,7 +1211,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>

</xml_diff>